<commit_message>
Consumo, Paneles e Inversores, se agregan con una modal
</commit_message>
<xml_diff>
--- a/public/docs/Calculo_de_Sistema_Fotovoltaico_Completo.xlsx
+++ b/public/docs/Calculo_de_Sistema_Fotovoltaico_Completo.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodrigos\Documents\projects\solar-calc\public\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7155"/>
   </bookViews>
@@ -10,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1160,63 +1165,6 @@
     <xf numFmtId="2" fontId="6" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1226,229 +1174,160 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="173" fontId="6" fillId="4" borderId="4" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="6" fillId="4" borderId="5" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="6" fillId="4" borderId="6" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="6" fillId="4" borderId="7" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="6" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="6" fillId="4" borderId="8" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="6" fillId="4" borderId="2" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="6" fillId="4" borderId="3" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="6" fillId="4" borderId="9" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="6" fillId="4" borderId="7" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="6" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="6" fillId="4" borderId="8" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="15" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="170" fontId="6" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="6" fillId="4" borderId="8" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="6" fillId="4" borderId="3" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="6" fillId="4" borderId="9" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="4" borderId="2" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="4" borderId="9" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="4" borderId="7" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="4" borderId="8" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="4" borderId="2" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="4" borderId="9" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="4" borderId="7" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="4" borderId="8" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="6" fillId="4" borderId="5" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="6" fillId="4" borderId="6" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="6" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="6" fillId="4" borderId="8" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="6" fillId="4" borderId="2" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="6" fillId="4" borderId="9" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="6" fillId="4" borderId="7" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="6" fillId="4" borderId="4" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="6" fillId="4" borderId="6" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="6" fillId="4" borderId="7" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="6" fillId="4" borderId="8" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="6" fillId="4" borderId="7" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="6" fillId="4" borderId="8" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="6" fillId="4" borderId="4" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="6" fillId="4" borderId="6" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="15" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="6" fillId="4" borderId="4" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="6" fillId="4" borderId="2" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="6" fillId="4" borderId="3" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="6" fillId="4" borderId="9" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="6" fillId="4" borderId="11" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="4" borderId="12" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="4" borderId="13" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="171" fontId="6" fillId="4" borderId="2" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1466,6 +1345,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="180" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1481,72 +1369,189 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="4" borderId="4" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="4" borderId="6" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="178" fontId="6" fillId="4" borderId="2" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="6" fillId="4" borderId="3" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="6" fillId="4" borderId="9" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="4" borderId="2" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="4" borderId="9" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="4" borderId="7" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="4" borderId="8" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="6" fillId="4" borderId="2" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="6" fillId="4" borderId="9" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="6" fillId="4" borderId="4" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="6" fillId="4" borderId="6" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="6" fillId="4" borderId="7" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="6" fillId="4" borderId="8" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="4" borderId="2" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="4" borderId="9" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="4" borderId="7" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="4" borderId="8" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="6" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="6" fillId="4" borderId="8" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="6" fillId="4" borderId="3" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="6" fillId="4" borderId="9" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="4" borderId="7" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="4" borderId="8" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="4" borderId="11" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="4" borderId="12" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="4" borderId="13" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="6" fillId="4" borderId="7" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="6" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="6" fillId="4" borderId="8" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="6" fillId="4" borderId="2" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="6" fillId="4" borderId="3" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="6" fillId="4" borderId="9" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Accent1" xfId="2" builtinId="29"/>
-    <cellStyle name="Good" xfId="3" builtinId="26"/>
+    <cellStyle name="Buena" xfId="3" builtinId="26"/>
+    <cellStyle name="Énfasis1" xfId="2" builtinId="29"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1816,7 +1821,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1826,11 +1831,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:O162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="M158" sqref="M158"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="F144" sqref="F144:H144"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.42578125" customWidth="1"/>
     <col min="3" max="4" width="6.85546875" customWidth="1"/>
@@ -1850,59 +1855,59 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="77" t="s">
+      <c r="B3" s="103" t="s">
         <v>150</v>
       </c>
-      <c r="C3" s="77"/>
-      <c r="D3" s="77"/>
-      <c r="E3" s="77"/>
-      <c r="F3" s="77"/>
-      <c r="G3" s="77"/>
-      <c r="H3" s="77"/>
-      <c r="I3" s="77"/>
-      <c r="J3" s="77"/>
-      <c r="K3" s="77"/>
-      <c r="L3" s="77"/>
-      <c r="M3" s="77"/>
-      <c r="N3" s="77"/>
-      <c r="O3" s="77"/>
+      <c r="C3" s="103"/>
+      <c r="D3" s="103"/>
+      <c r="E3" s="103"/>
+      <c r="F3" s="103"/>
+      <c r="G3" s="103"/>
+      <c r="H3" s="103"/>
+      <c r="I3" s="103"/>
+      <c r="J3" s="103"/>
+      <c r="K3" s="103"/>
+      <c r="L3" s="103"/>
+      <c r="M3" s="103"/>
+      <c r="N3" s="103"/>
+      <c r="O3" s="103"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="89">
+      <c r="C5" s="209">
         <v>-34.576653</v>
       </c>
-      <c r="D5" s="89"/>
-      <c r="F5" s="78" t="s">
+      <c r="D5" s="209"/>
+      <c r="F5" s="200" t="s">
         <v>158</v>
       </c>
-      <c r="G5" s="78"/>
-      <c r="H5" s="78" t="s">
+      <c r="G5" s="200"/>
+      <c r="H5" s="200" t="s">
         <v>157</v>
       </c>
-      <c r="I5" s="78"/>
-      <c r="J5" s="78"/>
-      <c r="K5" s="78"/>
-      <c r="L5" s="78"/>
-      <c r="M5" s="78"/>
-      <c r="N5" s="78"/>
+      <c r="I5" s="200"/>
+      <c r="J5" s="200"/>
+      <c r="K5" s="200"/>
+      <c r="L5" s="200"/>
+      <c r="M5" s="200"/>
+      <c r="N5" s="200"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="89">
+      <c r="C6" s="209">
         <v>-58.453485000000001</v>
       </c>
-      <c r="D6" s="89"/>
+      <c r="D6" s="209"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="86" t="s">
+      <c r="B8" s="141" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="88"/>
+      <c r="C8" s="143"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" s="23" t="s">
@@ -2257,44 +2262,44 @@
       </c>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B19" s="77" t="s">
+      <c r="B19" s="103" t="s">
         <v>151</v>
       </c>
-      <c r="C19" s="77"/>
-      <c r="D19" s="77"/>
-      <c r="E19" s="77"/>
-      <c r="F19" s="77"/>
-      <c r="G19" s="77"/>
-      <c r="H19" s="77"/>
-      <c r="I19" s="77"/>
-      <c r="J19" s="77"/>
-      <c r="K19" s="77"/>
-      <c r="L19" s="77"/>
-      <c r="M19" s="77"/>
-      <c r="N19" s="77"/>
-      <c r="O19" s="77"/>
+      <c r="C19" s="103"/>
+      <c r="D19" s="103"/>
+      <c r="E19" s="103"/>
+      <c r="F19" s="103"/>
+      <c r="G19" s="103"/>
+      <c r="H19" s="103"/>
+      <c r="I19" s="103"/>
+      <c r="J19" s="103"/>
+      <c r="K19" s="103"/>
+      <c r="L19" s="103"/>
+      <c r="M19" s="103"/>
+      <c r="N19" s="103"/>
+      <c r="O19" s="103"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B21" s="80" t="s">
+      <c r="B21" s="89" t="s">
         <v>131</v>
       </c>
-      <c r="C21" s="82"/>
-      <c r="D21" s="81"/>
-      <c r="I21" s="80" t="s">
+      <c r="C21" s="87"/>
+      <c r="D21" s="88"/>
+      <c r="I21" s="89" t="s">
         <v>134</v>
       </c>
-      <c r="J21" s="81"/>
-      <c r="K21" s="80" t="s">
+      <c r="J21" s="88"/>
+      <c r="K21" s="89" t="s">
         <v>135</v>
       </c>
-      <c r="L21" s="81"/>
+      <c r="L21" s="88"/>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B22" s="83" t="s">
+      <c r="B22" s="206" t="s">
         <v>132</v>
       </c>
-      <c r="C22" s="84"/>
-      <c r="D22" s="85"/>
+      <c r="C22" s="207"/>
+      <c r="D22" s="208"/>
       <c r="E22" s="25" t="s">
         <v>152</v>
       </c>
@@ -2321,11 +2326,11 @@
       </c>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B23" s="86" t="s">
+      <c r="B23" s="141" t="s">
         <v>136</v>
       </c>
-      <c r="C23" s="87"/>
-      <c r="D23" s="88"/>
+      <c r="C23" s="142"/>
+      <c r="D23" s="143"/>
       <c r="E23" s="65">
         <v>5</v>
       </c>
@@ -2356,11 +2361,11 @@
       </c>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B24" s="90" t="s">
+      <c r="B24" s="98" t="s">
         <v>137</v>
       </c>
-      <c r="C24" s="91"/>
-      <c r="D24" s="92"/>
+      <c r="C24" s="84"/>
+      <c r="D24" s="85"/>
       <c r="E24" s="67">
         <v>1</v>
       </c>
@@ -2391,11 +2396,11 @@
       </c>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B25" s="90" t="s">
+      <c r="B25" s="98" t="s">
         <v>138</v>
       </c>
-      <c r="C25" s="91"/>
-      <c r="D25" s="92"/>
+      <c r="C25" s="84"/>
+      <c r="D25" s="85"/>
       <c r="E25" s="67">
         <v>1</v>
       </c>
@@ -2426,11 +2431,11 @@
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B26" s="90" t="s">
+      <c r="B26" s="98" t="s">
         <v>139</v>
       </c>
-      <c r="C26" s="91"/>
-      <c r="D26" s="92"/>
+      <c r="C26" s="84"/>
+      <c r="D26" s="85"/>
       <c r="E26" s="67">
         <v>1</v>
       </c>
@@ -2461,11 +2466,11 @@
       </c>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B27" s="93" t="s">
+      <c r="B27" s="99" t="s">
         <v>140</v>
       </c>
-      <c r="C27" s="94"/>
-      <c r="D27" s="95"/>
+      <c r="C27" s="100"/>
+      <c r="D27" s="101"/>
       <c r="E27" s="69">
         <v>1</v>
       </c>
@@ -2496,28 +2501,28 @@
       </c>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B29" s="109" t="s">
+      <c r="B29" s="90" t="s">
         <v>143</v>
       </c>
-      <c r="C29" s="110"/>
-      <c r="D29" s="111"/>
-      <c r="E29" s="106">
+      <c r="C29" s="91"/>
+      <c r="D29" s="92"/>
+      <c r="E29" s="199">
         <f>SUM(G23:G27)</f>
         <v>275</v>
       </c>
-      <c r="F29" s="106"/>
+      <c r="F29" s="199"/>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B30" s="109" t="s">
+      <c r="B30" s="90" t="s">
         <v>144</v>
       </c>
-      <c r="C30" s="110"/>
-      <c r="D30" s="111"/>
-      <c r="E30" s="106">
+      <c r="C30" s="91"/>
+      <c r="D30" s="92"/>
+      <c r="E30" s="199">
         <f>SUM(H23:H27)</f>
         <v>835</v>
       </c>
-      <c r="F30" s="106"/>
+      <c r="F30" s="199"/>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B31" s="39" t="s">
@@ -2525,52 +2530,52 @@
       </c>
       <c r="C31" s="40"/>
       <c r="D31" s="41"/>
-      <c r="E31" s="107">
+      <c r="E31" s="201">
         <v>0.7</v>
       </c>
-      <c r="F31" s="108"/>
+      <c r="F31" s="202"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="78" t="s">
+      <c r="B33" s="200" t="s">
         <v>141</v>
       </c>
-      <c r="C33" s="78"/>
-      <c r="D33" s="78"/>
-      <c r="E33" s="78"/>
-      <c r="F33" s="78"/>
-      <c r="G33" s="79">
+      <c r="C33" s="200"/>
+      <c r="D33" s="200"/>
+      <c r="E33" s="200"/>
+      <c r="F33" s="200"/>
+      <c r="G33" s="198">
         <f>SUM(J23:J27)</f>
         <v>1570</v>
       </c>
-      <c r="H33" s="79"/>
+      <c r="H33" s="198"/>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B34" s="78" t="s">
+      <c r="B34" s="200" t="s">
         <v>142</v>
       </c>
-      <c r="C34" s="78"/>
-      <c r="D34" s="78"/>
-      <c r="E34" s="78"/>
-      <c r="F34" s="78"/>
-      <c r="G34" s="79">
+      <c r="C34" s="200"/>
+      <c r="D34" s="200"/>
+      <c r="E34" s="200"/>
+      <c r="F34" s="200"/>
+      <c r="G34" s="198">
         <f>SUM(L23:L27)</f>
         <v>1325</v>
       </c>
-      <c r="H34" s="79"/>
+      <c r="H34" s="198"/>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="109" t="s">
+      <c r="B36" s="90" t="s">
         <v>165</v>
       </c>
-      <c r="C36" s="110"/>
-      <c r="D36" s="110"/>
-      <c r="E36" s="110"/>
-      <c r="F36" s="111"/>
-      <c r="G36" s="120">
+      <c r="C36" s="91"/>
+      <c r="D36" s="91"/>
+      <c r="E36" s="91"/>
+      <c r="F36" s="92"/>
+      <c r="G36" s="187">
         <f>MAX(G33:H34)</f>
         <v>1570</v>
       </c>
-      <c r="H36" s="81"/>
+      <c r="H36" s="88"/>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" s="52"/>
@@ -2582,53 +2587,53 @@
       <c r="H37" s="30"/>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="80" t="s">
+      <c r="B38" s="89" t="s">
         <v>167</v>
       </c>
-      <c r="C38" s="82"/>
-      <c r="D38" s="81"/>
+      <c r="C38" s="87"/>
+      <c r="D38" s="88"/>
       <c r="E38" s="52"/>
       <c r="F38" s="52"/>
       <c r="G38" s="53"/>
       <c r="H38" s="30"/>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B39" s="122" t="s">
+      <c r="B39" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="C39" s="123"/>
-      <c r="D39" s="124"/>
-      <c r="E39" s="126">
+      <c r="C39" s="94"/>
+      <c r="D39" s="95"/>
+      <c r="E39" s="188">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F39" s="127"/>
+      <c r="F39" s="189"/>
       <c r="G39" s="53"/>
       <c r="H39" s="30"/>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="96" t="s">
+      <c r="B40" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="C40" s="97"/>
-      <c r="D40" s="98"/>
-      <c r="E40" s="128">
+      <c r="C40" s="78"/>
+      <c r="D40" s="79"/>
+      <c r="E40" s="190">
         <v>0.6</v>
       </c>
-      <c r="F40" s="129"/>
+      <c r="F40" s="191"/>
       <c r="G40" s="53"/>
       <c r="H40" s="30"/>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="112" t="s">
+      <c r="B41" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="C41" s="113"/>
-      <c r="D41" s="125"/>
-      <c r="E41" s="118">
+      <c r="C41" s="81"/>
+      <c r="D41" s="82"/>
+      <c r="E41" s="192">
         <f>G36*E39/E40</f>
         <v>2878.3333333333339</v>
       </c>
-      <c r="F41" s="119"/>
+      <c r="F41" s="193"/>
       <c r="G41" s="53"/>
       <c r="H41" s="30"/>
     </row>
@@ -2642,180 +2647,180 @@
       <c r="H42" s="30"/>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="80" t="s">
+      <c r="B43" s="89" t="s">
         <v>18</v>
       </c>
-      <c r="C43" s="82"/>
-      <c r="D43" s="81"/>
+      <c r="C43" s="87"/>
+      <c r="D43" s="88"/>
       <c r="E43" s="53"/>
       <c r="F43" s="53"/>
       <c r="G43" s="53"/>
       <c r="H43" s="30"/>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="122" t="s">
+      <c r="B44" s="93" t="s">
         <v>20</v>
       </c>
-      <c r="C44" s="123"/>
-      <c r="D44" s="123"/>
-      <c r="E44" s="114">
+      <c r="C44" s="94"/>
+      <c r="D44" s="94"/>
+      <c r="E44" s="168">
         <v>3</v>
       </c>
-      <c r="F44" s="115"/>
+      <c r="F44" s="169"/>
       <c r="G44" s="53"/>
       <c r="H44" s="30"/>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B45" s="96" t="s">
+      <c r="B45" s="77" t="s">
         <v>19</v>
       </c>
-      <c r="C45" s="97"/>
-      <c r="D45" s="97"/>
-      <c r="E45" s="116">
+      <c r="C45" s="78"/>
+      <c r="D45" s="78"/>
+      <c r="E45" s="203">
         <v>15</v>
       </c>
-      <c r="F45" s="117"/>
+      <c r="F45" s="204"/>
       <c r="G45" s="53"/>
       <c r="H45" s="30"/>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B46" s="112" t="s">
+      <c r="B46" s="80" t="s">
         <v>21</v>
       </c>
-      <c r="C46" s="113"/>
-      <c r="D46" s="113"/>
-      <c r="E46" s="118">
+      <c r="C46" s="81"/>
+      <c r="D46" s="81"/>
+      <c r="E46" s="192">
         <f>E41/E45*E44</f>
         <v>575.66666666666686</v>
       </c>
-      <c r="F46" s="119"/>
+      <c r="F46" s="193"/>
       <c r="G46" s="53"/>
       <c r="H46" s="30"/>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B48" s="109" t="s">
+      <c r="B48" s="90" t="s">
         <v>168</v>
       </c>
-      <c r="C48" s="110"/>
-      <c r="D48" s="110"/>
-      <c r="E48" s="110"/>
-      <c r="F48" s="111"/>
-      <c r="G48" s="120">
+      <c r="C48" s="91"/>
+      <c r="D48" s="91"/>
+      <c r="E48" s="91"/>
+      <c r="F48" s="92"/>
+      <c r="G48" s="187">
         <f>E46+E41</f>
         <v>3454.0000000000009</v>
       </c>
-      <c r="H48" s="121"/>
+      <c r="H48" s="205"/>
     </row>
     <row r="51" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B51" s="77" t="s">
+      <c r="B51" s="103" t="s">
         <v>160</v>
       </c>
-      <c r="C51" s="77"/>
-      <c r="D51" s="77"/>
-      <c r="E51" s="77"/>
-      <c r="F51" s="77"/>
-      <c r="G51" s="77"/>
-      <c r="H51" s="77"/>
-      <c r="I51" s="77"/>
-      <c r="J51" s="77"/>
-      <c r="K51" s="77"/>
-      <c r="L51" s="77"/>
-      <c r="M51" s="77"/>
-      <c r="N51" s="77"/>
-      <c r="O51" s="77"/>
+      <c r="C51" s="103"/>
+      <c r="D51" s="103"/>
+      <c r="E51" s="103"/>
+      <c r="F51" s="103"/>
+      <c r="G51" s="103"/>
+      <c r="H51" s="103"/>
+      <c r="I51" s="103"/>
+      <c r="J51" s="103"/>
+      <c r="K51" s="103"/>
+      <c r="L51" s="103"/>
+      <c r="M51" s="103"/>
+      <c r="N51" s="103"/>
+      <c r="O51" s="103"/>
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B53" s="80" t="s">
+      <c r="B53" s="89" t="s">
         <v>146</v>
       </c>
-      <c r="C53" s="81"/>
+      <c r="C53" s="88"/>
     </row>
     <row r="54" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B54" s="122" t="s">
+      <c r="B54" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="C54" s="123"/>
-      <c r="D54" s="123"/>
-      <c r="E54" s="124"/>
-      <c r="F54" s="104">
+      <c r="C54" s="94"/>
+      <c r="D54" s="94"/>
+      <c r="E54" s="95"/>
+      <c r="F54" s="196">
         <v>80</v>
       </c>
-      <c r="G54" s="104"/>
-      <c r="H54" s="105"/>
+      <c r="G54" s="196"/>
+      <c r="H54" s="197"/>
     </row>
     <row r="55" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B55" s="96" t="s">
+      <c r="B55" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="C55" s="97"/>
-      <c r="D55" s="97"/>
-      <c r="E55" s="98"/>
-      <c r="F55" s="102">
+      <c r="C55" s="78"/>
+      <c r="D55" s="78"/>
+      <c r="E55" s="79"/>
+      <c r="F55" s="116">
         <v>12</v>
       </c>
-      <c r="G55" s="102"/>
-      <c r="H55" s="103"/>
+      <c r="G55" s="116"/>
+      <c r="H55" s="117"/>
     </row>
     <row r="56" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B56" s="96" t="s">
+      <c r="B56" s="77" t="s">
         <v>145</v>
       </c>
-      <c r="C56" s="97"/>
-      <c r="D56" s="97"/>
-      <c r="E56" s="98"/>
-      <c r="F56" s="136">
+      <c r="C56" s="78"/>
+      <c r="D56" s="78"/>
+      <c r="E56" s="79"/>
+      <c r="F56" s="194">
         <v>5.01</v>
       </c>
-      <c r="G56" s="136"/>
-      <c r="H56" s="137"/>
+      <c r="G56" s="194"/>
+      <c r="H56" s="195"/>
     </row>
     <row r="57" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B57" s="96" t="s">
+      <c r="B57" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="C57" s="97"/>
-      <c r="D57" s="97"/>
-      <c r="E57" s="98"/>
-      <c r="F57" s="136">
+      <c r="C57" s="78"/>
+      <c r="D57" s="78"/>
+      <c r="E57" s="79"/>
+      <c r="F57" s="194">
         <v>4.5999999999999996</v>
       </c>
-      <c r="G57" s="136"/>
-      <c r="H57" s="137"/>
+      <c r="G57" s="194"/>
+      <c r="H57" s="195"/>
     </row>
     <row r="58" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B58" s="99" t="s">
+      <c r="B58" s="118" t="s">
         <v>147</v>
       </c>
-      <c r="C58" s="100"/>
-      <c r="D58" s="100"/>
-      <c r="E58" s="101"/>
-      <c r="F58" s="133" t="s">
+      <c r="C58" s="119"/>
+      <c r="D58" s="119"/>
+      <c r="E58" s="161"/>
+      <c r="F58" s="121" t="s">
         <v>148</v>
       </c>
-      <c r="G58" s="133"/>
-      <c r="H58" s="133"/>
+      <c r="G58" s="121"/>
+      <c r="H58" s="121"/>
     </row>
     <row r="59" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B59" s="130" t="s">
+      <c r="B59" s="104" t="s">
         <v>149</v>
       </c>
-      <c r="C59" s="131"/>
-      <c r="D59" s="131"/>
-      <c r="E59" s="132"/>
-      <c r="F59" s="134">
+      <c r="C59" s="105"/>
+      <c r="D59" s="105"/>
+      <c r="E59" s="164"/>
+      <c r="F59" s="107">
         <f>2859.74/8</f>
         <v>357.46749999999997</v>
       </c>
-      <c r="G59" s="134"/>
-      <c r="H59" s="135"/>
+      <c r="G59" s="107"/>
+      <c r="H59" s="108"/>
     </row>
     <row r="61" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B61" s="80" t="s">
+      <c r="B61" s="89" t="s">
         <v>161</v>
       </c>
-      <c r="C61" s="82"/>
-      <c r="D61" s="82"/>
-      <c r="E61" s="81"/>
+      <c r="C61" s="87"/>
+      <c r="D61" s="87"/>
+      <c r="E61" s="88"/>
     </row>
     <row r="62" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B62" s="23"/>
@@ -3064,24 +3069,24 @@
       </c>
     </row>
     <row r="68" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B68" s="80" t="s">
+      <c r="B68" s="89" t="s">
         <v>163</v>
       </c>
-      <c r="C68" s="82"/>
-      <c r="D68" s="82"/>
-      <c r="E68" s="88"/>
+      <c r="C68" s="87"/>
+      <c r="D68" s="87"/>
+      <c r="E68" s="143"/>
     </row>
     <row r="69" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B69" s="109" t="s">
+      <c r="B69" s="90" t="s">
         <v>164</v>
       </c>
-      <c r="C69" s="110"/>
-      <c r="D69" s="111"/>
-      <c r="E69" s="80">
+      <c r="C69" s="91"/>
+      <c r="D69" s="92"/>
+      <c r="E69" s="89">
         <f>ROUNDUP(G48/H66,0)</f>
         <v>16</v>
       </c>
-      <c r="F69" s="81"/>
+      <c r="F69" s="88"/>
     </row>
     <row r="70" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B70" s="8" t="s">
@@ -3089,11 +3094,11 @@
       </c>
       <c r="C70" s="9"/>
       <c r="D70" s="10"/>
-      <c r="E70" s="154">
+      <c r="E70" s="86">
         <f>E69*F59</f>
         <v>5719.48</v>
       </c>
-      <c r="F70" s="81"/>
+      <c r="F70" s="88"/>
     </row>
     <row r="71" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B71" s="6"/>
@@ -3110,36 +3115,36 @@
       <c r="F72" s="30"/>
     </row>
     <row r="73" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B73" s="144" t="s">
+      <c r="B73" s="178" t="s">
         <v>175</v>
       </c>
-      <c r="C73" s="144"/>
-      <c r="D73" s="144"/>
-      <c r="E73" s="144"/>
-      <c r="F73" s="144"/>
-      <c r="G73" s="144"/>
-      <c r="H73" s="144"/>
-      <c r="I73" s="144"/>
-      <c r="J73" s="144"/>
-      <c r="K73" s="144"/>
-      <c r="L73" s="144"/>
-      <c r="M73" s="144"/>
-      <c r="N73" s="144"/>
-      <c r="O73" s="144"/>
+      <c r="C73" s="178"/>
+      <c r="D73" s="178"/>
+      <c r="E73" s="178"/>
+      <c r="F73" s="178"/>
+      <c r="G73" s="178"/>
+      <c r="H73" s="178"/>
+      <c r="I73" s="178"/>
+      <c r="J73" s="178"/>
+      <c r="K73" s="178"/>
+      <c r="L73" s="178"/>
+      <c r="M73" s="178"/>
+      <c r="N73" s="178"/>
+      <c r="O73" s="178"/>
     </row>
     <row r="75" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B75" s="80" t="s">
+      <c r="B75" s="89" t="s">
         <v>173</v>
       </c>
-      <c r="C75" s="82"/>
-      <c r="D75" s="82"/>
-      <c r="E75" s="82"/>
-      <c r="F75" s="81"/>
-      <c r="G75" s="142">
+      <c r="C75" s="87"/>
+      <c r="D75" s="87"/>
+      <c r="E75" s="87"/>
+      <c r="F75" s="88"/>
+      <c r="G75" s="176">
         <f>E69*H65</f>
         <v>1280</v>
       </c>
-      <c r="H75" s="143"/>
+      <c r="H75" s="177"/>
     </row>
     <row r="76" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B76" s="52"/>
@@ -3151,64 +3156,64 @@
       <c r="H76" s="53"/>
     </row>
     <row r="77" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B77" s="80" t="s">
+      <c r="B77" s="89" t="s">
         <v>170</v>
       </c>
-      <c r="C77" s="82"/>
-      <c r="D77" s="82"/>
-      <c r="E77" s="81"/>
+      <c r="C77" s="87"/>
+      <c r="D77" s="87"/>
+      <c r="E77" s="88"/>
       <c r="F77" s="52"/>
       <c r="G77" s="53"/>
       <c r="H77" s="53"/>
     </row>
     <row r="78" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B78" s="80" t="s">
+      <c r="B78" s="89" t="s">
         <v>172</v>
       </c>
-      <c r="C78" s="81"/>
-      <c r="D78" s="80" t="s">
+      <c r="C78" s="88"/>
+      <c r="D78" s="89" t="s">
         <v>171</v>
       </c>
-      <c r="E78" s="81"/>
+      <c r="E78" s="88"/>
       <c r="F78" s="52"/>
       <c r="G78" s="53"/>
       <c r="H78" s="53"/>
     </row>
     <row r="79" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B79" s="150">
+      <c r="B79" s="183">
         <v>1000</v>
       </c>
-      <c r="C79" s="151"/>
-      <c r="D79" s="145">
+      <c r="C79" s="184"/>
+      <c r="D79" s="179">
         <v>12</v>
       </c>
-      <c r="E79" s="146"/>
+      <c r="E79" s="180"/>
       <c r="F79" s="52"/>
       <c r="G79" s="53"/>
       <c r="H79" s="53"/>
     </row>
     <row r="80" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B80" s="150">
+      <c r="B80" s="183">
         <v>5000</v>
       </c>
-      <c r="C80" s="151"/>
-      <c r="D80" s="147">
+      <c r="C80" s="184"/>
+      <c r="D80" s="115">
         <v>24</v>
       </c>
-      <c r="E80" s="103"/>
+      <c r="E80" s="117"/>
       <c r="F80" s="52"/>
       <c r="G80" s="53"/>
       <c r="H80" s="53"/>
     </row>
     <row r="81" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B81" s="152" t="s">
+      <c r="B81" s="185" t="s">
         <v>207</v>
       </c>
-      <c r="C81" s="153"/>
-      <c r="D81" s="148">
+      <c r="C81" s="186"/>
+      <c r="D81" s="181">
         <v>48</v>
       </c>
-      <c r="E81" s="149"/>
+      <c r="E81" s="182"/>
       <c r="F81" s="52"/>
       <c r="G81" s="53"/>
       <c r="H81" s="53"/>
@@ -3223,197 +3228,197 @@
       <c r="H82" s="53"/>
     </row>
     <row r="83" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B83" s="80" t="s">
+      <c r="B83" s="89" t="s">
         <v>174</v>
       </c>
-      <c r="C83" s="82"/>
-      <c r="D83" s="82"/>
-      <c r="E83" s="82"/>
-      <c r="F83" s="82"/>
-      <c r="G83" s="81"/>
-      <c r="H83" s="140">
+      <c r="C83" s="87"/>
+      <c r="D83" s="87"/>
+      <c r="E83" s="87"/>
+      <c r="F83" s="87"/>
+      <c r="G83" s="88"/>
+      <c r="H83" s="174">
         <f>IF(G75&lt;B79,D79,IF(G75&lt;B80,D80,D81))</f>
         <v>24</v>
       </c>
-      <c r="I83" s="141"/>
+      <c r="I83" s="175"/>
     </row>
     <row r="85" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B85" s="86" t="s">
+      <c r="B85" s="141" t="s">
         <v>6</v>
       </c>
-      <c r="C85" s="87"/>
-      <c r="D85" s="88"/>
+      <c r="C85" s="142"/>
+      <c r="D85" s="143"/>
     </row>
     <row r="86" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B86" s="109" t="s">
+      <c r="B86" s="90" t="s">
         <v>176</v>
       </c>
-      <c r="C86" s="110"/>
-      <c r="D86" s="110"/>
-      <c r="E86" s="111"/>
+      <c r="C86" s="91"/>
+      <c r="D86" s="91"/>
+      <c r="E86" s="92"/>
       <c r="F86" s="18">
         <f>ROUNDUP(H83/F55,0)</f>
         <v>2</v>
       </c>
     </row>
     <row r="87" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B87" s="109" t="s">
+      <c r="B87" s="90" t="s">
         <v>177</v>
       </c>
-      <c r="C87" s="110"/>
-      <c r="D87" s="110"/>
-      <c r="E87" s="111"/>
+      <c r="C87" s="91"/>
+      <c r="D87" s="91"/>
+      <c r="E87" s="92"/>
       <c r="F87" s="23">
         <f>ROUNDUP(E69/F86,0)</f>
         <v>8</v>
       </c>
     </row>
     <row r="89" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B89" s="86" t="s">
+      <c r="B89" s="141" t="s">
         <v>178</v>
       </c>
-      <c r="C89" s="87"/>
-      <c r="D89" s="88"/>
+      <c r="C89" s="142"/>
+      <c r="D89" s="143"/>
     </row>
     <row r="90" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B90" s="122" t="s">
+      <c r="B90" s="93" t="s">
         <v>8</v>
       </c>
-      <c r="C90" s="123"/>
-      <c r="D90" s="123"/>
-      <c r="E90" s="123"/>
-      <c r="F90" s="114">
+      <c r="C90" s="94"/>
+      <c r="D90" s="94"/>
+      <c r="E90" s="94"/>
+      <c r="F90" s="168">
         <v>3</v>
       </c>
-      <c r="G90" s="115"/>
+      <c r="G90" s="169"/>
     </row>
     <row r="91" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B91" s="96" t="s">
+      <c r="B91" s="77" t="s">
         <v>179</v>
       </c>
-      <c r="C91" s="97"/>
-      <c r="D91" s="97"/>
-      <c r="E91" s="97"/>
-      <c r="F91" s="155">
+      <c r="C91" s="78"/>
+      <c r="D91" s="78"/>
+      <c r="E91" s="78"/>
+      <c r="F91" s="170">
         <v>0.8</v>
       </c>
-      <c r="G91" s="156"/>
+      <c r="G91" s="171"/>
     </row>
     <row r="92" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B92" s="96" t="s">
+      <c r="B92" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="C92" s="97"/>
-      <c r="D92" s="97"/>
-      <c r="E92" s="97"/>
-      <c r="F92" s="155">
+      <c r="C92" s="78"/>
+      <c r="D92" s="78"/>
+      <c r="E92" s="78"/>
+      <c r="F92" s="170">
         <v>0.9</v>
       </c>
-      <c r="G92" s="156"/>
+      <c r="G92" s="171"/>
     </row>
     <row r="93" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B93" s="112" t="s">
+      <c r="B93" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="C93" s="113"/>
-      <c r="D93" s="113"/>
-      <c r="E93" s="113"/>
-      <c r="F93" s="157">
+      <c r="C93" s="81"/>
+      <c r="D93" s="81"/>
+      <c r="E93" s="81"/>
+      <c r="F93" s="162">
         <v>0.84</v>
       </c>
-      <c r="G93" s="158"/>
+      <c r="G93" s="163"/>
     </row>
     <row r="95" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B95" s="109" t="s">
+      <c r="B95" s="90" t="s">
         <v>7</v>
       </c>
-      <c r="C95" s="110"/>
-      <c r="D95" s="110"/>
-      <c r="E95" s="110"/>
-      <c r="F95" s="138">
+      <c r="C95" s="91"/>
+      <c r="D95" s="91"/>
+      <c r="E95" s="91"/>
+      <c r="F95" s="172">
         <f>(G36*(F90+1))/(H83*F91*F92*F93)</f>
         <v>432.64991181657837</v>
       </c>
-      <c r="G95" s="139"/>
+      <c r="G95" s="173"/>
     </row>
     <row r="97" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B97" s="80" t="s">
+      <c r="B97" s="89" t="s">
         <v>180</v>
       </c>
-      <c r="C97" s="82"/>
-      <c r="D97" s="81"/>
+      <c r="C97" s="87"/>
+      <c r="D97" s="88"/>
     </row>
     <row r="98" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B98" s="122" t="s">
+      <c r="B98" s="93" t="s">
         <v>11</v>
       </c>
-      <c r="C98" s="123"/>
-      <c r="D98" s="123"/>
-      <c r="E98" s="124"/>
-      <c r="F98" s="161">
+      <c r="C98" s="94"/>
+      <c r="D98" s="94"/>
+      <c r="E98" s="95"/>
+      <c r="F98" s="165">
         <v>220</v>
       </c>
-      <c r="G98" s="162"/>
-      <c r="H98" s="163"/>
+      <c r="G98" s="166"/>
+      <c r="H98" s="167"/>
     </row>
     <row r="99" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B99" s="96" t="s">
+      <c r="B99" s="77" t="s">
         <v>12</v>
       </c>
-      <c r="C99" s="97"/>
-      <c r="D99" s="97"/>
-      <c r="E99" s="98"/>
-      <c r="F99" s="147">
+      <c r="C99" s="78"/>
+      <c r="D99" s="78"/>
+      <c r="E99" s="79"/>
+      <c r="F99" s="115">
         <v>12</v>
       </c>
-      <c r="G99" s="102"/>
-      <c r="H99" s="103"/>
+      <c r="G99" s="116"/>
+      <c r="H99" s="117"/>
     </row>
     <row r="100" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B100" s="99" t="s">
+      <c r="B100" s="118" t="s">
         <v>147</v>
       </c>
-      <c r="C100" s="100"/>
-      <c r="D100" s="100"/>
-      <c r="E100" s="101"/>
-      <c r="F100" s="159" t="s">
+      <c r="C100" s="119"/>
+      <c r="D100" s="119"/>
+      <c r="E100" s="161"/>
+      <c r="F100" s="120" t="s">
         <v>184</v>
       </c>
-      <c r="G100" s="133"/>
-      <c r="H100" s="133"/>
+      <c r="G100" s="121"/>
+      <c r="H100" s="121"/>
     </row>
     <row r="101" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B101" s="130" t="s">
+      <c r="B101" s="104" t="s">
         <v>149</v>
       </c>
-      <c r="C101" s="131"/>
-      <c r="D101" s="131"/>
-      <c r="E101" s="132"/>
-      <c r="F101" s="160">
+      <c r="C101" s="105"/>
+      <c r="D101" s="105"/>
+      <c r="E101" s="164"/>
+      <c r="F101" s="106">
         <f>4406.82/8</f>
         <v>550.85249999999996</v>
       </c>
-      <c r="G101" s="134"/>
-      <c r="H101" s="135"/>
+      <c r="G101" s="107"/>
+      <c r="H101" s="108"/>
     </row>
     <row r="103" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B103" s="80" t="s">
+      <c r="B103" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="C103" s="82"/>
-      <c r="D103" s="81"/>
+      <c r="C103" s="87"/>
+      <c r="D103" s="88"/>
     </row>
     <row r="104" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B104" s="109" t="s">
+      <c r="B104" s="90" t="s">
         <v>164</v>
       </c>
-      <c r="C104" s="110"/>
-      <c r="D104" s="111"/>
-      <c r="E104" s="80">
+      <c r="C104" s="91"/>
+      <c r="D104" s="92"/>
+      <c r="E104" s="89">
         <f>ROUNDUP((H83*F95)/(F99*F98),0)</f>
         <v>4</v>
       </c>
-      <c r="F104" s="81"/>
+      <c r="F104" s="88"/>
       <c r="G104" s="30"/>
     </row>
     <row r="105" spans="2:8" x14ac:dyDescent="0.25">
@@ -3422,11 +3427,11 @@
       </c>
       <c r="C105" s="57"/>
       <c r="D105" s="58"/>
-      <c r="E105" s="164">
+      <c r="E105" s="157">
         <f>F110*F98</f>
         <v>440</v>
       </c>
-      <c r="F105" s="165"/>
+      <c r="F105" s="158"/>
       <c r="G105" s="30"/>
     </row>
     <row r="106" spans="2:8" x14ac:dyDescent="0.25">
@@ -3435,11 +3440,11 @@
       </c>
       <c r="C106" s="9"/>
       <c r="D106" s="10"/>
-      <c r="E106" s="154">
+      <c r="E106" s="86">
         <f>E104*F101</f>
         <v>2203.41</v>
       </c>
-      <c r="F106" s="81"/>
+      <c r="F106" s="88"/>
       <c r="G106" s="30"/>
     </row>
     <row r="107" spans="2:8" x14ac:dyDescent="0.25">
@@ -3451,19 +3456,19 @@
       <c r="G107" s="30"/>
     </row>
     <row r="108" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B108" s="80" t="s">
+      <c r="B108" s="89" t="s">
         <v>181</v>
       </c>
-      <c r="C108" s="82"/>
-      <c r="D108" s="81"/>
+      <c r="C108" s="87"/>
+      <c r="D108" s="88"/>
     </row>
     <row r="109" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B109" s="109" t="s">
+      <c r="B109" s="90" t="s">
         <v>182</v>
       </c>
-      <c r="C109" s="110"/>
-      <c r="D109" s="110"/>
-      <c r="E109" s="111"/>
+      <c r="C109" s="91"/>
+      <c r="D109" s="91"/>
+      <c r="E109" s="92"/>
       <c r="F109" s="23">
         <f>ROUNDUP(H83/F99, 0)</f>
         <v>2</v>
@@ -3471,12 +3476,12 @@
       <c r="G109" s="54"/>
     </row>
     <row r="110" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B110" s="109" t="s">
+      <c r="B110" s="90" t="s">
         <v>183</v>
       </c>
-      <c r="C110" s="110"/>
-      <c r="D110" s="110"/>
-      <c r="E110" s="111"/>
+      <c r="C110" s="91"/>
+      <c r="D110" s="91"/>
+      <c r="E110" s="92"/>
       <c r="F110" s="23">
         <f>ROUNDUP(E104/F109,0)</f>
         <v>2</v>
@@ -3484,47 +3489,47 @@
       <c r="G110" s="13"/>
     </row>
     <row r="112" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B112" s="86" t="s">
+      <c r="B112" s="141" t="s">
         <v>188</v>
       </c>
-      <c r="C112" s="87"/>
-      <c r="D112" s="88"/>
+      <c r="C112" s="142"/>
+      <c r="D112" s="143"/>
     </row>
     <row r="113" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B113" s="122" t="s">
+      <c r="B113" s="93" t="s">
         <v>186</v>
       </c>
-      <c r="C113" s="123"/>
-      <c r="D113" s="123"/>
-      <c r="E113" s="123"/>
-      <c r="F113" s="170">
+      <c r="C113" s="94"/>
+      <c r="D113" s="94"/>
+      <c r="E113" s="94"/>
+      <c r="F113" s="153">
         <f>1.25*F87*F57</f>
         <v>46</v>
       </c>
-      <c r="G113" s="171"/>
-      <c r="H113" s="80" t="str">
+      <c r="G113" s="154"/>
+      <c r="H113" s="89" t="str">
         <f>IF(F113&gt;F115,"ERROR. La coriente de carga supera el límite máximo C20","OK")</f>
         <v>OK</v>
       </c>
-      <c r="I113" s="81"/>
+      <c r="I113" s="88"/>
     </row>
     <row r="114" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B114" s="112" t="s">
+      <c r="B114" s="80" t="s">
         <v>187</v>
       </c>
-      <c r="C114" s="113"/>
-      <c r="D114" s="113"/>
-      <c r="E114" s="113"/>
-      <c r="F114" s="172">
+      <c r="C114" s="81"/>
+      <c r="D114" s="81"/>
+      <c r="E114" s="81"/>
+      <c r="F114" s="155">
         <f>(E29/E31)/(H83*F93)</f>
         <v>19.486961451247168</v>
       </c>
-      <c r="G114" s="173"/>
-      <c r="H114" s="80" t="str">
+      <c r="G114" s="156"/>
+      <c r="H114" s="89" t="str">
         <f>IF(F114&gt;F116,"ERROR. La corriente de descarga supera la corriente máxima de descarga C5","OK")</f>
         <v>OK</v>
       </c>
-      <c r="I114" s="81"/>
+      <c r="I114" s="88"/>
     </row>
     <row r="115" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B115" s="1" t="s">
@@ -3533,11 +3538,11 @@
       <c r="C115" s="2"/>
       <c r="D115" s="2"/>
       <c r="E115" s="2"/>
-      <c r="F115" s="170">
+      <c r="F115" s="153">
         <f>F98/5*F110</f>
         <v>88</v>
       </c>
-      <c r="G115" s="171"/>
+      <c r="G115" s="154"/>
     </row>
     <row r="116" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B116" s="3" t="s">
@@ -3546,49 +3551,49 @@
       <c r="C116" s="4"/>
       <c r="D116" s="4"/>
       <c r="E116" s="4"/>
-      <c r="F116" s="166">
+      <c r="F116" s="159">
         <f>F98/20*F110</f>
         <v>22</v>
       </c>
-      <c r="G116" s="167"/>
+      <c r="G116" s="160"/>
     </row>
     <row r="119" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B119" s="77" t="s">
+      <c r="B119" s="103" t="s">
         <v>191</v>
       </c>
-      <c r="C119" s="77"/>
-      <c r="D119" s="77"/>
-      <c r="E119" s="77"/>
-      <c r="F119" s="77"/>
-      <c r="G119" s="77"/>
-      <c r="H119" s="77"/>
-      <c r="I119" s="77"/>
-      <c r="J119" s="77"/>
-      <c r="K119" s="77"/>
-      <c r="L119" s="77"/>
-      <c r="M119" s="77"/>
-      <c r="N119" s="77"/>
-      <c r="O119" s="77"/>
+      <c r="C119" s="103"/>
+      <c r="D119" s="103"/>
+      <c r="E119" s="103"/>
+      <c r="F119" s="103"/>
+      <c r="G119" s="103"/>
+      <c r="H119" s="103"/>
+      <c r="I119" s="103"/>
+      <c r="J119" s="103"/>
+      <c r="K119" s="103"/>
+      <c r="L119" s="103"/>
+      <c r="M119" s="103"/>
+      <c r="N119" s="103"/>
+      <c r="O119" s="103"/>
     </row>
     <row r="121" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B121" s="80" t="s">
+      <c r="B121" s="89" t="s">
         <v>13</v>
       </c>
-      <c r="C121" s="82"/>
-      <c r="D121" s="81"/>
+      <c r="C121" s="87"/>
+      <c r="D121" s="88"/>
     </row>
     <row r="122" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B122" s="109" t="s">
+      <c r="B122" s="90" t="s">
         <v>14</v>
       </c>
-      <c r="C122" s="110"/>
-      <c r="D122" s="110"/>
-      <c r="E122" s="111"/>
-      <c r="F122" s="168">
+      <c r="C122" s="91"/>
+      <c r="D122" s="91"/>
+      <c r="E122" s="92"/>
+      <c r="F122" s="151">
         <f>1.25*(F87*F56)</f>
         <v>50.099999999999994</v>
       </c>
-      <c r="G122" s="169"/>
+      <c r="G122" s="152"/>
       <c r="I122" s="74" t="s">
         <v>208</v>
       </c>
@@ -3601,134 +3606,134 @@
       <c r="G123" s="60"/>
     </row>
     <row r="124" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B124" s="80" t="s">
+      <c r="B124" s="89" t="s">
         <v>194</v>
       </c>
-      <c r="C124" s="82"/>
-      <c r="D124" s="81"/>
+      <c r="C124" s="87"/>
+      <c r="D124" s="88"/>
       <c r="E124" s="52"/>
       <c r="F124" s="60"/>
       <c r="G124" s="60"/>
     </row>
     <row r="125" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B125" s="177" t="s">
+      <c r="B125" s="135" t="s">
         <v>193</v>
       </c>
-      <c r="C125" s="178"/>
-      <c r="D125" s="178"/>
-      <c r="E125" s="179"/>
-      <c r="F125" s="174">
+      <c r="C125" s="136"/>
+      <c r="D125" s="136"/>
+      <c r="E125" s="137"/>
+      <c r="F125" s="132">
         <v>40</v>
       </c>
-      <c r="G125" s="175"/>
-      <c r="H125" s="176"/>
+      <c r="G125" s="133"/>
+      <c r="H125" s="134"/>
     </row>
     <row r="126" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B126" s="180" t="s">
+      <c r="B126" s="138" t="s">
         <v>147</v>
       </c>
-      <c r="C126" s="181"/>
-      <c r="D126" s="181"/>
-      <c r="E126" s="182"/>
-      <c r="F126" s="188" t="s">
+      <c r="C126" s="139"/>
+      <c r="D126" s="139"/>
+      <c r="E126" s="140"/>
+      <c r="F126" s="149" t="s">
         <v>192</v>
       </c>
-      <c r="G126" s="189"/>
-      <c r="H126" s="133"/>
+      <c r="G126" s="150"/>
+      <c r="H126" s="121"/>
     </row>
     <row r="127" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B127" s="185" t="s">
+      <c r="B127" s="146" t="s">
         <v>149</v>
       </c>
-      <c r="C127" s="186"/>
-      <c r="D127" s="186"/>
-      <c r="E127" s="187"/>
-      <c r="F127" s="160">
+      <c r="C127" s="147"/>
+      <c r="D127" s="147"/>
+      <c r="E127" s="148"/>
+      <c r="F127" s="106">
         <f>1741.48/8</f>
         <v>217.685</v>
       </c>
-      <c r="G127" s="134"/>
-      <c r="H127" s="135"/>
+      <c r="G127" s="107"/>
+      <c r="H127" s="108"/>
     </row>
     <row r="128" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B128" s="194" t="s">
+      <c r="B128" s="126" t="s">
         <v>133</v>
       </c>
-      <c r="C128" s="195"/>
-      <c r="D128" s="195"/>
-      <c r="E128" s="196"/>
-      <c r="F128" s="197">
+      <c r="C128" s="127"/>
+      <c r="D128" s="127"/>
+      <c r="E128" s="128"/>
+      <c r="F128" s="129">
         <v>1</v>
       </c>
-      <c r="G128" s="198"/>
-      <c r="H128" s="199"/>
+      <c r="G128" s="130"/>
+      <c r="H128" s="131"/>
     </row>
     <row r="129" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B129" s="177" t="s">
+      <c r="B129" s="135" t="s">
         <v>193</v>
       </c>
-      <c r="C129" s="178"/>
-      <c r="D129" s="178"/>
-      <c r="E129" s="179"/>
-      <c r="F129" s="174">
+      <c r="C129" s="136"/>
+      <c r="D129" s="136"/>
+      <c r="E129" s="137"/>
+      <c r="F129" s="132">
         <v>20</v>
       </c>
-      <c r="G129" s="175"/>
-      <c r="H129" s="176"/>
+      <c r="G129" s="133"/>
+      <c r="H129" s="134"/>
     </row>
     <row r="130" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B130" s="180" t="s">
+      <c r="B130" s="138" t="s">
         <v>147</v>
       </c>
-      <c r="C130" s="181"/>
-      <c r="D130" s="181"/>
-      <c r="E130" s="182"/>
-      <c r="F130" s="188" t="s">
+      <c r="C130" s="139"/>
+      <c r="D130" s="139"/>
+      <c r="E130" s="140"/>
+      <c r="F130" s="149" t="s">
         <v>195</v>
       </c>
-      <c r="G130" s="189"/>
-      <c r="H130" s="133"/>
+      <c r="G130" s="150"/>
+      <c r="H130" s="121"/>
     </row>
     <row r="131" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B131" s="185" t="s">
+      <c r="B131" s="146" t="s">
         <v>149</v>
       </c>
-      <c r="C131" s="186"/>
-      <c r="D131" s="186"/>
-      <c r="E131" s="187"/>
-      <c r="F131" s="160">
+      <c r="C131" s="147"/>
+      <c r="D131" s="147"/>
+      <c r="E131" s="148"/>
+      <c r="F131" s="106">
         <f>1135.94/8</f>
         <v>141.99250000000001</v>
       </c>
-      <c r="G131" s="134"/>
-      <c r="H131" s="135"/>
+      <c r="G131" s="107"/>
+      <c r="H131" s="108"/>
     </row>
     <row r="132" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B132" s="194" t="s">
+      <c r="B132" s="126" t="s">
         <v>133</v>
       </c>
-      <c r="C132" s="195"/>
-      <c r="D132" s="195"/>
-      <c r="E132" s="196"/>
-      <c r="F132" s="197">
+      <c r="C132" s="127"/>
+      <c r="D132" s="127"/>
+      <c r="E132" s="128"/>
+      <c r="F132" s="129">
         <v>1</v>
       </c>
-      <c r="G132" s="198"/>
-      <c r="H132" s="199"/>
+      <c r="G132" s="130"/>
+      <c r="H132" s="131"/>
     </row>
     <row r="133" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B133" s="194" t="s">
+      <c r="B133" s="126" t="s">
         <v>169</v>
       </c>
-      <c r="C133" s="195"/>
-      <c r="D133" s="195"/>
-      <c r="E133" s="196"/>
-      <c r="F133" s="154">
+      <c r="C133" s="127"/>
+      <c r="D133" s="127"/>
+      <c r="E133" s="128"/>
+      <c r="F133" s="86">
         <f>F131*F132+F127*F128</f>
         <v>359.67750000000001</v>
       </c>
-      <c r="G133" s="192"/>
-      <c r="H133" s="193"/>
+      <c r="G133" s="124"/>
+      <c r="H133" s="125"/>
     </row>
     <row r="134" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B134" s="61"/>
@@ -3740,268 +3745,268 @@
       <c r="H134" s="59"/>
     </row>
     <row r="135" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B135" s="86" t="s">
+      <c r="B135" s="141" t="s">
         <v>15</v>
       </c>
-      <c r="C135" s="87"/>
-      <c r="D135" s="88"/>
+      <c r="C135" s="142"/>
+      <c r="D135" s="143"/>
     </row>
     <row r="136" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B136" s="109" t="s">
+      <c r="B136" s="90" t="s">
         <v>16</v>
       </c>
-      <c r="C136" s="110"/>
-      <c r="D136" s="110"/>
-      <c r="E136" s="111"/>
-      <c r="F136" s="183">
+      <c r="C136" s="91"/>
+      <c r="D136" s="91"/>
+      <c r="E136" s="92"/>
+      <c r="F136" s="144">
         <f>E29*1.25/E31</f>
         <v>491.07142857142861</v>
       </c>
-      <c r="G136" s="184"/>
+      <c r="G136" s="145"/>
     </row>
     <row r="137" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B137" s="109" t="s">
+      <c r="B137" s="90" t="s">
         <v>196</v>
       </c>
-      <c r="C137" s="110"/>
-      <c r="D137" s="110"/>
-      <c r="E137" s="111"/>
-      <c r="F137" s="190">
+      <c r="C137" s="91"/>
+      <c r="D137" s="91"/>
+      <c r="E137" s="92"/>
+      <c r="F137" s="122">
         <f>(E30)/(220*E31)</f>
         <v>5.4220779220779223</v>
       </c>
-      <c r="G137" s="191"/>
+      <c r="G137" s="123"/>
     </row>
     <row r="139" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B139" s="80" t="s">
+      <c r="B139" s="89" t="s">
         <v>197</v>
       </c>
-      <c r="C139" s="82"/>
-      <c r="D139" s="81"/>
+      <c r="C139" s="87"/>
+      <c r="D139" s="88"/>
     </row>
     <row r="140" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B140" s="122" t="s">
+      <c r="B140" s="93" t="s">
         <v>198</v>
       </c>
-      <c r="C140" s="123"/>
-      <c r="D140" s="123"/>
-      <c r="E140" s="123"/>
-      <c r="F140" s="204">
+      <c r="C140" s="94"/>
+      <c r="D140" s="94"/>
+      <c r="E140" s="94"/>
+      <c r="F140" s="112">
         <v>600</v>
       </c>
-      <c r="G140" s="205"/>
-      <c r="H140" s="206"/>
-      <c r="I140" s="80" t="str">
+      <c r="G140" s="113"/>
+      <c r="H140" s="114"/>
+      <c r="I140" s="89" t="str">
         <f>IF(F136&gt;F140,"ERROR. La potencia requerida es mayor a la que puede dar el inversor","OK")</f>
         <v>OK</v>
       </c>
-      <c r="J140" s="81"/>
+      <c r="J140" s="88"/>
     </row>
     <row r="141" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B141" s="96" t="s">
+      <c r="B141" s="77" t="s">
         <v>199</v>
       </c>
-      <c r="C141" s="97"/>
-      <c r="D141" s="97"/>
-      <c r="E141" s="97"/>
-      <c r="F141" s="147">
+      <c r="C141" s="78"/>
+      <c r="D141" s="78"/>
+      <c r="E141" s="78"/>
+      <c r="F141" s="115">
         <v>24</v>
       </c>
-      <c r="G141" s="102"/>
-      <c r="H141" s="103"/>
+      <c r="G141" s="116"/>
+      <c r="H141" s="117"/>
     </row>
     <row r="142" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B142" s="96" t="s">
+      <c r="B142" s="77" t="s">
         <v>201</v>
       </c>
-      <c r="C142" s="97"/>
-      <c r="D142" s="97"/>
-      <c r="E142" s="98"/>
-      <c r="F142" s="201">
+      <c r="C142" s="78"/>
+      <c r="D142" s="78"/>
+      <c r="E142" s="79"/>
+      <c r="F142" s="109">
         <v>11</v>
       </c>
-      <c r="G142" s="202"/>
-      <c r="H142" s="203"/>
-      <c r="I142" s="80" t="str">
+      <c r="G142" s="110"/>
+      <c r="H142" s="111"/>
+      <c r="I142" s="89" t="str">
         <f>IF(F137&gt;F142,"ERROR. La corriente de salida es mayor a la que puede soportar el inversor","OK")</f>
         <v>OK</v>
       </c>
-      <c r="J142" s="81"/>
+      <c r="J142" s="88"/>
     </row>
     <row r="143" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B143" s="99" t="s">
+      <c r="B143" s="118" t="s">
         <v>147</v>
       </c>
-      <c r="C143" s="100"/>
-      <c r="D143" s="100"/>
-      <c r="E143" s="100"/>
-      <c r="F143" s="159" t="s">
+      <c r="C143" s="119"/>
+      <c r="D143" s="119"/>
+      <c r="E143" s="119"/>
+      <c r="F143" s="120" t="s">
         <v>200</v>
       </c>
-      <c r="G143" s="133"/>
-      <c r="H143" s="133"/>
+      <c r="G143" s="121"/>
+      <c r="H143" s="121"/>
     </row>
     <row r="144" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B144" s="130" t="s">
+      <c r="B144" s="104" t="s">
         <v>149</v>
       </c>
-      <c r="C144" s="131"/>
-      <c r="D144" s="131"/>
-      <c r="E144" s="131"/>
-      <c r="F144" s="160">
+      <c r="C144" s="105"/>
+      <c r="D144" s="105"/>
+      <c r="E144" s="105"/>
+      <c r="F144" s="106">
         <f>7981.16/8</f>
         <v>997.64499999999998</v>
       </c>
-      <c r="G144" s="134"/>
-      <c r="H144" s="135"/>
+      <c r="G144" s="107"/>
+      <c r="H144" s="108"/>
     </row>
     <row r="147" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B147" s="77" t="s">
+      <c r="B147" s="103" t="s">
         <v>202</v>
       </c>
-      <c r="C147" s="77"/>
-      <c r="D147" s="77"/>
-      <c r="E147" s="77"/>
-      <c r="F147" s="77"/>
-      <c r="G147" s="77"/>
-      <c r="H147" s="77"/>
-      <c r="I147" s="77"/>
-      <c r="J147" s="77"/>
-      <c r="K147" s="77"/>
-      <c r="L147" s="77"/>
-      <c r="M147" s="77"/>
-      <c r="N147" s="77"/>
-      <c r="O147" s="77"/>
+      <c r="C147" s="103"/>
+      <c r="D147" s="103"/>
+      <c r="E147" s="103"/>
+      <c r="F147" s="103"/>
+      <c r="G147" s="103"/>
+      <c r="H147" s="103"/>
+      <c r="I147" s="103"/>
+      <c r="J147" s="103"/>
+      <c r="K147" s="103"/>
+      <c r="L147" s="103"/>
+      <c r="M147" s="103"/>
+      <c r="N147" s="103"/>
+      <c r="O147" s="103"/>
     </row>
     <row r="149" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B149" s="109" t="s">
+      <c r="B149" s="90" t="s">
         <v>204</v>
       </c>
-      <c r="C149" s="110"/>
-      <c r="D149" s="111"/>
-      <c r="E149" s="80" t="s">
+      <c r="C149" s="91"/>
+      <c r="D149" s="92"/>
+      <c r="E149" s="89" t="s">
         <v>147</v>
       </c>
-      <c r="F149" s="82"/>
-      <c r="G149" s="81"/>
-      <c r="H149" s="80" t="s">
+      <c r="F149" s="87"/>
+      <c r="G149" s="88"/>
+      <c r="H149" s="89" t="s">
         <v>133</v>
       </c>
-      <c r="I149" s="81"/>
-      <c r="J149" s="80" t="s">
+      <c r="I149" s="88"/>
+      <c r="J149" s="89" t="s">
         <v>205</v>
       </c>
-      <c r="K149" s="82"/>
-      <c r="L149" s="81"/>
+      <c r="K149" s="87"/>
+      <c r="L149" s="88"/>
       <c r="M149" s="55"/>
       <c r="N149" s="54"/>
       <c r="O149" s="54"/>
     </row>
     <row r="150" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B150" s="96" t="s">
+      <c r="B150" s="77" t="s">
         <v>203</v>
       </c>
-      <c r="C150" s="97"/>
-      <c r="D150" s="98"/>
-      <c r="E150" s="90" t="str">
+      <c r="C150" s="78"/>
+      <c r="D150" s="79"/>
+      <c r="E150" s="98" t="str">
         <f>F58</f>
         <v>Solartec KS80T - SL*</v>
       </c>
-      <c r="F150" s="91"/>
-      <c r="G150" s="92"/>
-      <c r="H150" s="90">
+      <c r="F150" s="84"/>
+      <c r="G150" s="85"/>
+      <c r="H150" s="98">
         <f>E69</f>
         <v>16</v>
       </c>
-      <c r="I150" s="92"/>
-      <c r="J150" s="200">
+      <c r="I150" s="85"/>
+      <c r="J150" s="83">
         <f>E70</f>
         <v>5719.48</v>
       </c>
-      <c r="K150" s="91"/>
-      <c r="L150" s="92"/>
+      <c r="K150" s="84"/>
+      <c r="L150" s="85"/>
       <c r="M150" s="62">
         <f t="shared" ref="M150:M153" si="5">J150/$J$155</f>
         <v>0.61630916317918361</v>
       </c>
     </row>
     <row r="151" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B151" s="96" t="s">
+      <c r="B151" s="77" t="s">
         <v>206</v>
       </c>
-      <c r="C151" s="97"/>
-      <c r="D151" s="98"/>
-      <c r="E151" s="90" t="str">
+      <c r="C151" s="78"/>
+      <c r="D151" s="79"/>
+      <c r="E151" s="98" t="str">
         <f>F100</f>
         <v>Moura CLEAN 12MF220</v>
       </c>
-      <c r="F151" s="91"/>
-      <c r="G151" s="92"/>
-      <c r="H151" s="90">
+      <c r="F151" s="84"/>
+      <c r="G151" s="85"/>
+      <c r="H151" s="98">
         <f>E104</f>
         <v>4</v>
       </c>
-      <c r="I151" s="92"/>
-      <c r="J151" s="200">
+      <c r="I151" s="85"/>
+      <c r="J151" s="83">
         <f>E106</f>
         <v>2203.41</v>
       </c>
-      <c r="K151" s="91"/>
-      <c r="L151" s="92"/>
+      <c r="K151" s="84"/>
+      <c r="L151" s="85"/>
       <c r="M151" s="63">
         <f t="shared" si="5"/>
         <v>0.23743098555124681</v>
       </c>
     </row>
     <row r="152" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B152" s="96" t="s">
+      <c r="B152" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="C152" s="97"/>
-      <c r="D152" s="98"/>
-      <c r="E152" s="90" t="str">
+      <c r="C152" s="78"/>
+      <c r="D152" s="79"/>
+      <c r="E152" s="98" t="str">
         <f>F126</f>
         <v>SOLARTEC SC40</v>
       </c>
-      <c r="F152" s="91"/>
-      <c r="G152" s="92"/>
-      <c r="H152" s="90">
+      <c r="F152" s="84"/>
+      <c r="G152" s="85"/>
+      <c r="H152" s="98">
         <v>1</v>
       </c>
-      <c r="I152" s="92"/>
-      <c r="J152" s="200">
+      <c r="I152" s="85"/>
+      <c r="J152" s="83">
         <f>F127</f>
         <v>217.685</v>
       </c>
-      <c r="K152" s="207"/>
-      <c r="L152" s="208"/>
+      <c r="K152" s="96"/>
+      <c r="L152" s="97"/>
       <c r="M152" s="63">
         <f t="shared" si="5"/>
         <v>2.3456898212190724E-2</v>
       </c>
     </row>
     <row r="153" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B153" s="96" t="s">
+      <c r="B153" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="C153" s="97"/>
-      <c r="D153" s="98"/>
-      <c r="E153" s="90" t="str">
+      <c r="C153" s="78"/>
+      <c r="D153" s="79"/>
+      <c r="E153" s="98" t="str">
         <f>F130</f>
         <v>SOLARTEC SC20</v>
       </c>
-      <c r="F153" s="91"/>
-      <c r="G153" s="92"/>
-      <c r="H153" s="90">
+      <c r="F153" s="84"/>
+      <c r="G153" s="85"/>
+      <c r="H153" s="98">
         <v>1</v>
       </c>
-      <c r="I153" s="92"/>
-      <c r="J153" s="200">
+      <c r="I153" s="85"/>
+      <c r="J153" s="83">
         <f>F131</f>
         <v>141.99250000000001</v>
       </c>
-      <c r="K153" s="207"/>
-      <c r="L153" s="208"/>
+      <c r="K153" s="96"/>
+      <c r="L153" s="97"/>
       <c r="M153" s="63">
         <f t="shared" si="5"/>
         <v>1.5300565585109178E-2</v>
@@ -4013,152 +4018,277 @@
       </c>
       <c r="C154" s="4"/>
       <c r="D154" s="5"/>
-      <c r="E154" s="93" t="str">
+      <c r="E154" s="99" t="str">
         <f>F143</f>
         <v>TGP 24 600</v>
       </c>
-      <c r="F154" s="94"/>
-      <c r="G154" s="95"/>
-      <c r="H154" s="93">
+      <c r="F154" s="100"/>
+      <c r="G154" s="101"/>
+      <c r="H154" s="99">
         <v>1</v>
       </c>
-      <c r="I154" s="95"/>
-      <c r="J154" s="209">
+      <c r="I154" s="101"/>
+      <c r="J154" s="102">
         <f>F144</f>
         <v>997.64499999999998</v>
       </c>
-      <c r="K154" s="94"/>
-      <c r="L154" s="95"/>
+      <c r="K154" s="100"/>
+      <c r="L154" s="101"/>
       <c r="M154" s="64">
         <f>J154/$J$155</f>
         <v>0.10750238747226963</v>
       </c>
     </row>
     <row r="155" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="J155" s="154">
+      <c r="J155" s="86">
         <f>SUM(J150:L154)</f>
         <v>9280.2124999999996</v>
       </c>
-      <c r="K155" s="82"/>
-      <c r="L155" s="81"/>
+      <c r="K155" s="87"/>
+      <c r="L155" s="88"/>
     </row>
     <row r="157" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B157" s="109" t="s">
+      <c r="B157" s="90" t="s">
         <v>204</v>
       </c>
-      <c r="C157" s="110"/>
-      <c r="D157" s="110"/>
-      <c r="E157" s="110"/>
-      <c r="F157" s="110"/>
-      <c r="G157" s="110"/>
-      <c r="H157" s="110"/>
-      <c r="I157" s="111"/>
-      <c r="J157" s="80" t="s">
+      <c r="C157" s="91"/>
+      <c r="D157" s="91"/>
+      <c r="E157" s="91"/>
+      <c r="F157" s="91"/>
+      <c r="G157" s="91"/>
+      <c r="H157" s="91"/>
+      <c r="I157" s="92"/>
+      <c r="J157" s="89" t="s">
         <v>205</v>
       </c>
-      <c r="K157" s="82"/>
-      <c r="L157" s="81"/>
+      <c r="K157" s="87"/>
+      <c r="L157" s="88"/>
     </row>
     <row r="158" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B158" s="122" t="s">
+      <c r="B158" s="93" t="s">
         <v>209</v>
       </c>
-      <c r="C158" s="123"/>
-      <c r="D158" s="123"/>
-      <c r="E158" s="123"/>
-      <c r="F158" s="123"/>
-      <c r="G158" s="123"/>
-      <c r="H158" s="123"/>
-      <c r="I158" s="124"/>
-      <c r="J158" s="200">
+      <c r="C158" s="94"/>
+      <c r="D158" s="94"/>
+      <c r="E158" s="94"/>
+      <c r="F158" s="94"/>
+      <c r="G158" s="94"/>
+      <c r="H158" s="94"/>
+      <c r="I158" s="95"/>
+      <c r="J158" s="83">
         <v>650</v>
       </c>
-      <c r="K158" s="91"/>
-      <c r="L158" s="92"/>
+      <c r="K158" s="84"/>
+      <c r="L158" s="85"/>
     </row>
     <row r="159" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B159" s="96" t="s">
+      <c r="B159" s="77" t="s">
         <v>210</v>
       </c>
-      <c r="C159" s="97"/>
-      <c r="D159" s="97"/>
-      <c r="E159" s="97"/>
-      <c r="F159" s="97"/>
-      <c r="G159" s="97"/>
-      <c r="H159" s="97"/>
-      <c r="I159" s="98"/>
-      <c r="J159" s="200">
+      <c r="C159" s="78"/>
+      <c r="D159" s="78"/>
+      <c r="E159" s="78"/>
+      <c r="F159" s="78"/>
+      <c r="G159" s="78"/>
+      <c r="H159" s="78"/>
+      <c r="I159" s="79"/>
+      <c r="J159" s="83">
         <v>550</v>
       </c>
-      <c r="K159" s="91"/>
-      <c r="L159" s="92"/>
+      <c r="K159" s="84"/>
+      <c r="L159" s="85"/>
     </row>
     <row r="160" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B160" s="96" t="s">
+      <c r="B160" s="77" t="s">
         <v>211</v>
       </c>
-      <c r="C160" s="97"/>
-      <c r="D160" s="97"/>
-      <c r="E160" s="97"/>
-      <c r="F160" s="97"/>
-      <c r="G160" s="97"/>
-      <c r="H160" s="97"/>
-      <c r="I160" s="98"/>
-      <c r="J160" s="200">
+      <c r="C160" s="78"/>
+      <c r="D160" s="78"/>
+      <c r="E160" s="78"/>
+      <c r="F160" s="78"/>
+      <c r="G160" s="78"/>
+      <c r="H160" s="78"/>
+      <c r="I160" s="79"/>
+      <c r="J160" s="83">
         <v>800</v>
       </c>
-      <c r="K160" s="91"/>
-      <c r="L160" s="92"/>
+      <c r="K160" s="84"/>
+      <c r="L160" s="85"/>
     </row>
     <row r="161" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B161" s="112" t="s">
+      <c r="B161" s="80" t="s">
         <v>212</v>
       </c>
-      <c r="C161" s="113"/>
-      <c r="D161" s="113"/>
-      <c r="E161" s="113"/>
-      <c r="F161" s="113"/>
-      <c r="G161" s="113"/>
-      <c r="H161" s="113"/>
-      <c r="I161" s="125"/>
-      <c r="J161" s="200">
+      <c r="C161" s="81"/>
+      <c r="D161" s="81"/>
+      <c r="E161" s="81"/>
+      <c r="F161" s="81"/>
+      <c r="G161" s="81"/>
+      <c r="H161" s="81"/>
+      <c r="I161" s="82"/>
+      <c r="J161" s="83">
         <v>1400</v>
       </c>
-      <c r="K161" s="91"/>
-      <c r="L161" s="92"/>
+      <c r="K161" s="84"/>
+      <c r="L161" s="85"/>
     </row>
     <row r="162" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="J162" s="154">
+      <c r="J162" s="86">
         <f>SUM(J158:L161)</f>
         <v>3400</v>
       </c>
-      <c r="K162" s="82"/>
-      <c r="L162" s="81"/>
+      <c r="K162" s="87"/>
+      <c r="L162" s="88"/>
     </row>
   </sheetData>
   <mergeCells count="193">
-    <mergeCell ref="B160:I160"/>
-    <mergeCell ref="B161:I161"/>
-    <mergeCell ref="J158:L158"/>
-    <mergeCell ref="J159:L159"/>
-    <mergeCell ref="J160:L160"/>
-    <mergeCell ref="J161:L161"/>
-    <mergeCell ref="J162:L162"/>
-    <mergeCell ref="J157:L157"/>
-    <mergeCell ref="B157:I157"/>
-    <mergeCell ref="B158:I158"/>
-    <mergeCell ref="B159:I159"/>
-    <mergeCell ref="J155:L155"/>
-    <mergeCell ref="B153:D153"/>
-    <mergeCell ref="J152:L152"/>
-    <mergeCell ref="J153:L153"/>
-    <mergeCell ref="H152:I152"/>
-    <mergeCell ref="H153:I153"/>
-    <mergeCell ref="E154:G154"/>
-    <mergeCell ref="H154:I154"/>
-    <mergeCell ref="J154:L154"/>
-    <mergeCell ref="E153:G153"/>
-    <mergeCell ref="E152:G152"/>
+    <mergeCell ref="B19:O19"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:N5"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="B3:O3"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="F92:G92"/>
+    <mergeCell ref="B95:E95"/>
+    <mergeCell ref="B92:E92"/>
+    <mergeCell ref="B61:E61"/>
+    <mergeCell ref="B36:F36"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="B59:E59"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="F58:H58"/>
+    <mergeCell ref="F59:H59"/>
+    <mergeCell ref="F57:H57"/>
+    <mergeCell ref="F56:H56"/>
+    <mergeCell ref="B51:O51"/>
+    <mergeCell ref="B54:E54"/>
+    <mergeCell ref="B55:E55"/>
+    <mergeCell ref="B56:E56"/>
+    <mergeCell ref="B57:E57"/>
+    <mergeCell ref="H83:I83"/>
+    <mergeCell ref="B75:F75"/>
+    <mergeCell ref="G75:H75"/>
+    <mergeCell ref="B73:O73"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="D78:E78"/>
+    <mergeCell ref="D79:E79"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="B68:E68"/>
+    <mergeCell ref="E69:F69"/>
+    <mergeCell ref="E70:F70"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="F90:G90"/>
+    <mergeCell ref="F91:G91"/>
+    <mergeCell ref="B90:E90"/>
+    <mergeCell ref="B91:E91"/>
+    <mergeCell ref="B85:D85"/>
+    <mergeCell ref="B86:E86"/>
+    <mergeCell ref="B87:E87"/>
+    <mergeCell ref="B89:D89"/>
+    <mergeCell ref="B77:E77"/>
+    <mergeCell ref="B83:G83"/>
+    <mergeCell ref="B58:E58"/>
+    <mergeCell ref="F55:H55"/>
+    <mergeCell ref="F54:H54"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="B48:F48"/>
+    <mergeCell ref="B97:D97"/>
+    <mergeCell ref="B100:E100"/>
+    <mergeCell ref="F93:G93"/>
+    <mergeCell ref="B93:E93"/>
+    <mergeCell ref="E104:F104"/>
+    <mergeCell ref="F100:H100"/>
+    <mergeCell ref="B101:E101"/>
+    <mergeCell ref="F101:H101"/>
+    <mergeCell ref="F98:H98"/>
+    <mergeCell ref="F99:H99"/>
+    <mergeCell ref="B104:D104"/>
+    <mergeCell ref="F95:G95"/>
+    <mergeCell ref="E106:F106"/>
+    <mergeCell ref="B103:D103"/>
+    <mergeCell ref="E105:F105"/>
+    <mergeCell ref="B108:D108"/>
+    <mergeCell ref="B109:E109"/>
+    <mergeCell ref="B110:E110"/>
+    <mergeCell ref="B98:E98"/>
+    <mergeCell ref="B99:E99"/>
+    <mergeCell ref="F116:G116"/>
+    <mergeCell ref="H113:I113"/>
+    <mergeCell ref="H114:I114"/>
+    <mergeCell ref="B119:O119"/>
+    <mergeCell ref="F122:G122"/>
+    <mergeCell ref="B122:E122"/>
+    <mergeCell ref="B121:D121"/>
+    <mergeCell ref="B112:D112"/>
+    <mergeCell ref="B113:E113"/>
+    <mergeCell ref="B114:E114"/>
+    <mergeCell ref="F113:G113"/>
+    <mergeCell ref="F114:G114"/>
+    <mergeCell ref="F115:G115"/>
+    <mergeCell ref="F125:H125"/>
+    <mergeCell ref="B125:E125"/>
+    <mergeCell ref="B126:E126"/>
+    <mergeCell ref="B124:D124"/>
+    <mergeCell ref="B129:E129"/>
+    <mergeCell ref="F129:H129"/>
+    <mergeCell ref="B135:D135"/>
+    <mergeCell ref="F136:G136"/>
+    <mergeCell ref="B136:E136"/>
+    <mergeCell ref="B127:E127"/>
+    <mergeCell ref="F127:H127"/>
+    <mergeCell ref="F126:H126"/>
+    <mergeCell ref="B130:E130"/>
+    <mergeCell ref="F130:H130"/>
+    <mergeCell ref="B131:E131"/>
+    <mergeCell ref="F131:H131"/>
+    <mergeCell ref="B143:E143"/>
+    <mergeCell ref="F143:H143"/>
+    <mergeCell ref="F137:G137"/>
+    <mergeCell ref="B137:E137"/>
+    <mergeCell ref="B139:D139"/>
+    <mergeCell ref="F133:H133"/>
+    <mergeCell ref="B133:E133"/>
+    <mergeCell ref="F128:H128"/>
+    <mergeCell ref="B128:E128"/>
+    <mergeCell ref="B132:E132"/>
+    <mergeCell ref="F132:H132"/>
     <mergeCell ref="E149:G149"/>
     <mergeCell ref="E150:G150"/>
     <mergeCell ref="E151:G151"/>
@@ -4183,153 +4313,28 @@
     <mergeCell ref="F140:H140"/>
     <mergeCell ref="B141:E141"/>
     <mergeCell ref="F141:H141"/>
-    <mergeCell ref="B143:E143"/>
-    <mergeCell ref="F143:H143"/>
-    <mergeCell ref="F137:G137"/>
-    <mergeCell ref="B137:E137"/>
-    <mergeCell ref="B139:D139"/>
-    <mergeCell ref="F133:H133"/>
-    <mergeCell ref="B133:E133"/>
-    <mergeCell ref="F128:H128"/>
-    <mergeCell ref="B128:E128"/>
-    <mergeCell ref="B132:E132"/>
-    <mergeCell ref="F132:H132"/>
-    <mergeCell ref="F125:H125"/>
-    <mergeCell ref="B125:E125"/>
-    <mergeCell ref="B126:E126"/>
-    <mergeCell ref="B124:D124"/>
-    <mergeCell ref="B129:E129"/>
-    <mergeCell ref="F129:H129"/>
-    <mergeCell ref="B135:D135"/>
-    <mergeCell ref="F136:G136"/>
-    <mergeCell ref="B136:E136"/>
-    <mergeCell ref="B127:E127"/>
-    <mergeCell ref="F127:H127"/>
-    <mergeCell ref="F126:H126"/>
-    <mergeCell ref="B130:E130"/>
-    <mergeCell ref="F130:H130"/>
-    <mergeCell ref="B131:E131"/>
-    <mergeCell ref="F131:H131"/>
-    <mergeCell ref="H113:I113"/>
-    <mergeCell ref="H114:I114"/>
-    <mergeCell ref="B119:O119"/>
-    <mergeCell ref="F122:G122"/>
-    <mergeCell ref="B122:E122"/>
-    <mergeCell ref="B121:D121"/>
-    <mergeCell ref="B112:D112"/>
-    <mergeCell ref="B113:E113"/>
-    <mergeCell ref="B114:E114"/>
-    <mergeCell ref="F113:G113"/>
-    <mergeCell ref="F114:G114"/>
-    <mergeCell ref="F115:G115"/>
-    <mergeCell ref="E106:F106"/>
-    <mergeCell ref="B103:D103"/>
-    <mergeCell ref="E105:F105"/>
-    <mergeCell ref="B108:D108"/>
-    <mergeCell ref="B109:E109"/>
-    <mergeCell ref="B110:E110"/>
-    <mergeCell ref="B98:E98"/>
-    <mergeCell ref="B99:E99"/>
-    <mergeCell ref="F116:G116"/>
-    <mergeCell ref="B97:D97"/>
-    <mergeCell ref="B100:E100"/>
-    <mergeCell ref="F93:G93"/>
-    <mergeCell ref="B93:E93"/>
-    <mergeCell ref="E104:F104"/>
-    <mergeCell ref="F100:H100"/>
-    <mergeCell ref="B101:E101"/>
-    <mergeCell ref="F101:H101"/>
-    <mergeCell ref="F98:H98"/>
-    <mergeCell ref="F99:H99"/>
-    <mergeCell ref="B104:D104"/>
-    <mergeCell ref="B69:D69"/>
-    <mergeCell ref="B68:E68"/>
-    <mergeCell ref="E69:F69"/>
-    <mergeCell ref="E70:F70"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="F90:G90"/>
-    <mergeCell ref="F91:G91"/>
-    <mergeCell ref="B90:E90"/>
-    <mergeCell ref="B91:E91"/>
-    <mergeCell ref="B85:D85"/>
-    <mergeCell ref="B86:E86"/>
-    <mergeCell ref="B87:E87"/>
-    <mergeCell ref="F95:G95"/>
-    <mergeCell ref="B89:D89"/>
-    <mergeCell ref="B77:E77"/>
-    <mergeCell ref="B83:G83"/>
-    <mergeCell ref="H83:I83"/>
-    <mergeCell ref="B75:F75"/>
-    <mergeCell ref="G75:H75"/>
-    <mergeCell ref="B73:O73"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="D78:E78"/>
-    <mergeCell ref="D79:E79"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="F92:G92"/>
-    <mergeCell ref="B95:E95"/>
-    <mergeCell ref="B92:E92"/>
-    <mergeCell ref="B61:E61"/>
-    <mergeCell ref="B36:F36"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="B59:E59"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="F58:H58"/>
-    <mergeCell ref="F59:H59"/>
-    <mergeCell ref="F57:H57"/>
-    <mergeCell ref="F56:H56"/>
-    <mergeCell ref="B51:O51"/>
-    <mergeCell ref="B54:E54"/>
-    <mergeCell ref="B55:E55"/>
-    <mergeCell ref="B56:E56"/>
-    <mergeCell ref="B57:E57"/>
-    <mergeCell ref="B58:E58"/>
-    <mergeCell ref="F55:H55"/>
-    <mergeCell ref="F54:H54"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="B33:F33"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="G48:H48"/>
-    <mergeCell ref="B48:F48"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B19:O19"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:N5"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="B3:O3"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="J155:L155"/>
+    <mergeCell ref="B153:D153"/>
+    <mergeCell ref="J152:L152"/>
+    <mergeCell ref="J153:L153"/>
+    <mergeCell ref="H152:I152"/>
+    <mergeCell ref="H153:I153"/>
+    <mergeCell ref="E154:G154"/>
+    <mergeCell ref="H154:I154"/>
+    <mergeCell ref="J154:L154"/>
+    <mergeCell ref="E153:G153"/>
+    <mergeCell ref="E152:G152"/>
+    <mergeCell ref="B160:I160"/>
+    <mergeCell ref="B161:I161"/>
+    <mergeCell ref="J158:L158"/>
+    <mergeCell ref="J159:L159"/>
+    <mergeCell ref="J160:L160"/>
+    <mergeCell ref="J161:L161"/>
+    <mergeCell ref="J162:L162"/>
+    <mergeCell ref="J157:L157"/>
+    <mergeCell ref="B157:I157"/>
+    <mergeCell ref="B158:I158"/>
+    <mergeCell ref="B159:I159"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -4344,7 +4349,7 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="6" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F6" s="11" t="s">

</xml_diff>